<commit_message>
Atualizacao dos artefatos do 15 ao 20
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Poison\Desktop\ACS\OPE\Artefatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Poison\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -166,9 +166,6 @@
     <t>Gerente verifica produto</t>
   </si>
   <si>
-    <t>Gerentesolicita devolução ou troca</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gerente devolve produto </t>
   </si>
   <si>
@@ -193,13 +190,16 @@
     <t>Gerente recusa proposta</t>
   </si>
   <si>
-    <t>Escritório da Gerencia - Atender cliente</t>
-  </si>
-  <si>
     <t>Gerente recebe convidados</t>
   </si>
   <si>
     <t>OBS: Outras planilhas no menu abaixo</t>
+  </si>
+  <si>
+    <t>Escritório da Gerencia - Fechar contrato</t>
+  </si>
+  <si>
+    <t>Escritório da Gerencia - Realizar evento</t>
   </si>
 </sst>
 </file>
@@ -238,7 +238,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +305,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -538,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -564,52 +570,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -624,46 +675,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -690,6 +705,12 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -699,17 +720,50 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -722,45 +776,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -786,6 +801,986 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>454268</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>8792</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>414703</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>27842</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="454268" y="3503734"/>
+          <a:ext cx="1271954" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Salão - Atender cliente</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>65941</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>8792</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1337895</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>27842</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Retângulo 6">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1995789" y="3504053"/>
+          <a:ext cx="1271954" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Balcão - Atender cliente</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>732307</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>8792</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>310585</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>27842</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Retângulo 7">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5073702" y="3518003"/>
+          <a:ext cx="1272725" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Escritório da Gerência - Compra</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>56485</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>11322</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1333855</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>30372</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Retângulo 8">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1986551" y="4473033"/>
+          <a:ext cx="1277370" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Escritório da Gerência - Devolução ou troca</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>734921</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>16119</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>308621</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>35169</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Retângulo 9">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5075008" y="4463880"/>
+          <a:ext cx="1271635" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Escritório da Gerência - Realizar</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> evento</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1606506</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>16119</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>468221</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>35169</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Retângulo 10">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3536354" y="4463880"/>
+          <a:ext cx="1271954" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Escritório da Gerência - Fechar contrato</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>438977</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>8793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>399412</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>27843</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Retângulo 11">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="438977" y="4456554"/>
+          <a:ext cx="1277370" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Escritório da Gerência - Solicitar cancelamento</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1592437</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>16337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>461966</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>35387</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Retângulo 12">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3522503" y="3525548"/>
+          <a:ext cx="1280858" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Cozinha - Preparar pedido</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Seta para a Esquerda 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="4000500"/>
+          <a:ext cx="1552575" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1" i="1"/>
+            <a:t>VOLTAR</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="1" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>16566</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>157370</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>343315</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>71645</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Seta para a Esquerda 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="629479" y="2161761"/>
+          <a:ext cx="1552575" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1" i="1"/>
+            <a:t>VOLTAR</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="1" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Seta para a Esquerda 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="3733800"/>
+          <a:ext cx="1552575" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1" i="1"/>
+            <a:t>VOLTAR</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="1" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Seta para a Esquerda 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1285875" y="2276475"/>
+          <a:ext cx="1552575" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1" i="1"/>
+            <a:t>VOLTAR</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="1" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Seta para a Esquerda 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1409700" y="2247900"/>
+          <a:ext cx="1552575" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1" i="1"/>
+            <a:t>VOLTAR</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="1" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16565</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>149086</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>956227</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>63361</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Seta para a Esquerda 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1242391" y="2824369"/>
+          <a:ext cx="1552575" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1" i="1"/>
+            <a:t>VOLTAR</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="1" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Seta para a Esquerda 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1485900" y="1952625"/>
+          <a:ext cx="1552575" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1" i="1"/>
+            <a:t>VOLTAR</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="1" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1077,12 +2072,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="36.140625" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
@@ -1093,10 +2089,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1123,10 +2119,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="38" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3">
@@ -1135,18 +2131,18 @@
       <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="3">
         <v>2</v>
       </c>
@@ -1156,33 +2152,33 @@
       <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="3">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="3">
         <v>4</v>
       </c>
@@ -1193,14 +2189,14 @@
         <v>13</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="18"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="3">
         <v>5</v>
       </c>
@@ -1211,14 +2207,14 @@
         <v>23</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="13"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="3">
         <v>6</v>
       </c>
@@ -1229,14 +2225,14 @@
         <v>24</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="18"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="34"/>
+      <c r="B8" s="36" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="3">
@@ -1245,51 +2241,55 @@
       <c r="D8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="20" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="18"/>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="13"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="3">
         <v>8</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="20" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="18"/>
+      <c r="J9" s="11"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
+      <c r="A11" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A11:D11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B2:B7"/>
+    <mergeCell ref="A11:G11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1297,12 +2297,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
     <col min="4" max="4" width="35.85546875" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
@@ -1311,11 +2312,11 @@
     <col min="10" max="10" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1342,10 +2343,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="38" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3">
@@ -1354,18 +2355,18 @@
       <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="3">
         <v>2</v>
       </c>
@@ -1375,33 +2376,33 @@
       <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="3">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="3">
         <v>4</v>
       </c>
@@ -1412,14 +2413,14 @@
         <v>13</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="18"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="3">
         <v>5</v>
       </c>
@@ -1430,14 +2431,14 @@
         <v>23</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="13"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="3">
         <v>6</v>
       </c>
@@ -1448,14 +2449,14 @@
         <v>24</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="18"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="41"/>
+      <c r="B8" s="36" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="3">
@@ -1464,32 +2465,32 @@
       <c r="D8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="20" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="18"/>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="13"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="3">
         <v>8</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="20" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="18"/>
+      <c r="J9" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1499,6 +2500,7 @@
     <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1506,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,112 +2524,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="17">
         <v>1</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="37"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="42"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32">
+      <c r="A3" s="44"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="17">
         <v>2</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32">
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="17">
         <v>3</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="37"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42"/>
-      <c r="B5" s="29" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="17">
         <v>7</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="41" t="s">
+      <c r="E5" s="19"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="37"/>
+      <c r="J5" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1636,6 +2638,7 @@
     <mergeCell ref="B2:B4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1643,12 +2646,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
@@ -1658,10 +2662,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="46"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1688,10 +2692,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="38" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3">
@@ -1700,18 +2704,18 @@
       <c r="D2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="3">
         <v>2</v>
       </c>
@@ -1721,33 +2725,33 @@
       <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="3">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="3">
         <v>4</v>
       </c>
@@ -1758,14 +2762,14 @@
         <v>13</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="18"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="45"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="3">
         <v>5</v>
       </c>
@@ -1776,14 +2780,14 @@
         <v>23</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="48"/>
+      <c r="B7" s="36" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3">
@@ -1792,32 +2796,32 @@
       <c r="D7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="20" t="s">
+      <c r="E7" s="9"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="18"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="3">
         <v>7</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="20" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="18"/>
+      <c r="J8" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1827,6 +2831,7 @@
     <mergeCell ref="B7:B8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1834,13 +2839,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="32.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
@@ -1851,10 +2856,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="46"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1881,10 +2886,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="38" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3">
@@ -1893,18 +2898,18 @@
       <c r="D2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="3">
         <v>2</v>
       </c>
@@ -1914,15 +2919,15 @@
       <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="36" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="3">
@@ -1931,32 +2936,32 @@
       <c r="D4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="20" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="18"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
-      <c r="B5" s="13"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="3">
         <v>7</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="20" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="18"/>
+      <c r="J5" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1966,6 +2971,7 @@
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1973,13 +2979,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="33.140625" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
@@ -1989,112 +2995,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="17">
         <v>1</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="37"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32">
+      <c r="A3" s="53"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="17">
         <v>2</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="53"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="17">
+        <v>3</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="53"/>
+      <c r="B5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="17">
+        <v>7</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32">
-        <v>3</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="37"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50"/>
-      <c r="B5" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="32">
-        <v>7</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="37"/>
+      <c r="J5" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2103,6 +3109,7 @@
     <mergeCell ref="B2:B4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2111,11 +3118,12 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="A1:J7"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="34.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
@@ -2126,10 +3134,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2156,118 +3164,118 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="38" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="16"/>
+        <v>48</v>
+      </c>
+      <c r="E2" s="9"/>
       <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="55"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="3">
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="55"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="27"/>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="3">
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="55"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="3">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="55"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="27"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="57"/>
+      <c r="B6" s="36" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="3">
         <v>7</v>
       </c>
-      <c r="D6" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20" t="s">
+      <c r="D6" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="55"/>
+      <c r="J6" s="27"/>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="53"/>
-      <c r="B7" s="13"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="3">
         <v>8</v>
       </c>
-      <c r="D7" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20" t="s">
+      <c r="D7" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="55"/>
+      <c r="J7" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2277,6 +3285,7 @@
     <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2285,12 +3294,12 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="4" max="4" width="30.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
@@ -2302,10 +3311,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2332,8 +3341,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
-        <v>55</v>
+      <c r="A2" s="71" t="s">
+        <v>57</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>9</v>
@@ -2342,42 +3351,42 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="16"/>
+        <v>54</v>
+      </c>
+      <c r="E2" s="9"/>
       <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="55"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="72"/>
+      <c r="B3" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="72"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="69"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="73"/>
+      <c r="A4" s="73"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2390,5 +3399,6 @@
     <mergeCell ref="C3:D4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>